<commit_message>
Some report and Collection dropdown work
</commit_message>
<xml_diff>
--- a/Documentation/Test plan.xlsx
+++ b/Documentation/Test plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darryllrobinson/Documents/projects/thesystem/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A07C9118-47B2-4B43-8ABA-D67B19DA1CC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0ED116-B845-204A-BD1B-7640DE842D48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{6323BECF-22C4-8E4C-B1D9-E828BE35501A}"/>
   </bookViews>
@@ -32,6 +32,119 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <t>Pend</t>
+  </si>
+  <si>
+    <t>CIPC Status</t>
+  </si>
+  <si>
+    <t>Account Status</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>Number called</t>
+  </si>
+  <si>
+    <t>Person contacted</t>
+  </si>
+  <si>
+    <t>Email used</t>
+  </si>
+  <si>
+    <t>PTP Date</t>
+  </si>
+  <si>
+    <t>PTP Amount</t>
+  </si>
+  <si>
+    <t>Outcome resolution</t>
+  </si>
+  <si>
+    <t>Debit date</t>
+  </si>
+  <si>
+    <t>Debit amount</t>
+  </si>
+  <si>
+    <t>Pend reason</t>
+  </si>
+  <si>
+    <t>Outcome notes</t>
+  </si>
+  <si>
+    <t>NVDT</t>
+  </si>
+  <si>
+    <t>Assignment</t>
+  </si>
+  <si>
+    <t>Next steps</t>
+  </si>
+  <si>
+    <t>Final dereg</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>MR XX</t>
+  </si>
+  <si>
+    <t>10/30/2020 12:00 AM</t>
+  </si>
+  <si>
+    <t>callback</t>
+  </si>
+  <si>
+    <t>no notes because</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>Big ones</t>
+  </si>
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>BAC101</t>
+  </si>
+  <si>
+    <t>Option 2</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Joe Soap</t>
+  </si>
+  <si>
+    <t>nnnnn</t>
+  </si>
+  <si>
+    <t>10/23/2020 2:00 AM</t>
+  </si>
+  <si>
+    <t>dgdgdgdgdgdggdgdgdgd</t>
+  </si>
+  <si>
+    <t>dispute</t>
+  </si>
+  <si>
+    <t>Call</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -43,12 +156,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,8 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,12 +508,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCCB4E9-16BD-0841-824A-3E15E291EBF5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1234</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="3">
+        <v>43962.208333333336</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3">
+        <v>1112345678</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1">
+        <v>43962</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>